<commit_message>
change graph for M2.1a
</commit_message>
<xml_diff>
--- a/IO_M2.1_new/M2.1a_outputs/M2.1a_TablesAndGraphs Sep2016(1).xlsx
+++ b/IO_M2.1_new/M2.1a_outputs/M2.1a_TablesAndGraphs Sep2016(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="885" windowWidth="28800" windowHeight="13335" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="885" windowWidth="28800" windowHeight="13335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="28" r:id="rId1"/>
@@ -1327,9 +1327,6 @@
 (40% funded ratio or less)</t>
   </si>
   <si>
-    <t>Probability that, anytime in 30 years, there will be</t>
-  </si>
-  <si>
     <t>Asset-to-payroll ratio and net cash flow
 (Median across 1,000 simulations)</t>
   </si>
@@ -1343,6 +1340,9 @@
   </si>
   <si>
     <t>Plan demographic characteristics and risks of underfunding and of high employer contributions</t>
+  </si>
+  <si>
+    <t>Probability (%) that, anytime in 30 years, there will be</t>
   </si>
 </sst>
 </file>
@@ -1854,17 +1854,17 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="16" fillId="7" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="3" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1890,23 +1890,23 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -10868,153 +10868,153 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
     </row>
     <row r="4" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="115"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="117"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="115"/>
-      <c r="S5" s="115"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="117"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="117"/>
+      <c r="R6" s="117"/>
+      <c r="S6" s="117"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="116" t="s">
+      <c r="D8" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="116" t="s">
+      <c r="E8" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="116" t="s">
+      <c r="H8" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="116" t="s">
+      <c r="I8" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="116" t="s">
+      <c r="J8" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="116" t="s">
+      <c r="K8" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="116" t="s">
+      <c r="L8" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="116" t="s">
+      <c r="M8" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="116" t="s">
+      <c r="N8" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="116" t="s">
+      <c r="O8" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="116" t="s">
+      <c r="P8" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="116" t="s">
+      <c r="Q8" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="R8" s="116" t="s">
+      <c r="R8" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="S8" s="116" t="s">
+      <c r="S8" s="119" t="s">
         <v>45</v>
       </c>
     </row>
@@ -11078,99 +11078,110 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="115"/>
-      <c r="N10" s="115"/>
-      <c r="O10" s="115"/>
-      <c r="P10" s="115"/>
-      <c r="Q10" s="115"/>
-      <c r="R10" s="115"/>
-      <c r="S10" s="115"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="117"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="117"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="117"/>
+      <c r="M10" s="117"/>
+      <c r="N10" s="117"/>
+      <c r="O10" s="117"/>
+      <c r="P10" s="117"/>
+      <c r="Q10" s="117"/>
+      <c r="R10" s="117"/>
+      <c r="S10" s="117"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="114" t="s">
+      <c r="A11" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="115"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="115"/>
-      <c r="L11" s="115"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="115"/>
-      <c r="P11" s="115"/>
-      <c r="Q11" s="115"/>
-      <c r="R11" s="115"/>
-      <c r="S11" s="115"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="117"/>
+      <c r="N11" s="117"/>
+      <c r="O11" s="117"/>
+      <c r="P11" s="117"/>
+      <c r="Q11" s="117"/>
+      <c r="R11" s="117"/>
+      <c r="S11" s="117"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="115"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="115"/>
-      <c r="R12" s="115"/>
-      <c r="S12" s="115"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="117"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="117"/>
+      <c r="P12" s="117"/>
+      <c r="Q12" s="117"/>
+      <c r="R12" s="117"/>
+      <c r="S12" s="117"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="114" t="s">
+      <c r="A13" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="115"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="115"/>
-      <c r="Q13" s="115"/>
-      <c r="R13" s="115"/>
-      <c r="S13" s="115"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="117"/>
+      <c r="P13" s="117"/>
+      <c r="Q13" s="117"/>
+      <c r="R13" s="117"/>
+      <c r="S13" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A13:S13"/>
+    <mergeCell ref="M8"/>
+    <mergeCell ref="N8"/>
+    <mergeCell ref="O8"/>
+    <mergeCell ref="P8"/>
+    <mergeCell ref="Q8"/>
+    <mergeCell ref="L8"/>
+    <mergeCell ref="S8"/>
+    <mergeCell ref="A10:S10"/>
+    <mergeCell ref="A11:S11"/>
+    <mergeCell ref="A12:S12"/>
     <mergeCell ref="A3:S3"/>
     <mergeCell ref="A4:S4"/>
     <mergeCell ref="A5:S5"/>
@@ -11187,17 +11198,6 @@
     <mergeCell ref="I8"/>
     <mergeCell ref="J8"/>
     <mergeCell ref="K8"/>
-    <mergeCell ref="A13:S13"/>
-    <mergeCell ref="M8"/>
-    <mergeCell ref="N8"/>
-    <mergeCell ref="O8"/>
-    <mergeCell ref="P8"/>
-    <mergeCell ref="Q8"/>
-    <mergeCell ref="L8"/>
-    <mergeCell ref="S8"/>
-    <mergeCell ref="A10:S10"/>
-    <mergeCell ref="A11:S11"/>
-    <mergeCell ref="A12:S12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
@@ -11239,356 +11239,356 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="116" t="s">
         <v>273</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="115"/>
-      <c r="AB3" s="115"/>
-      <c r="AC3" s="115"/>
-      <c r="AD3" s="115"/>
-      <c r="AE3" s="115"/>
-      <c r="AF3" s="115"/>
-      <c r="AG3" s="115"/>
-      <c r="AH3" s="115"/>
-      <c r="AI3" s="115"/>
-      <c r="AJ3" s="115"/>
-      <c r="AK3" s="115"/>
-      <c r="AL3" s="115"/>
-      <c r="AM3" s="115"/>
-      <c r="AN3" s="115"/>
-      <c r="AO3" s="115"/>
-      <c r="AP3" s="115"/>
-      <c r="AQ3" s="115"/>
-      <c r="AR3" s="115"/>
-      <c r="AS3" s="115"/>
-      <c r="AT3" s="115"/>
-      <c r="AU3" s="115"/>
-      <c r="AV3" s="115"/>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="117"/>
+      <c r="P3" s="117"/>
+      <c r="Q3" s="117"/>
+      <c r="R3" s="117"/>
+      <c r="S3" s="117"/>
+      <c r="T3" s="117"/>
+      <c r="U3" s="117"/>
+      <c r="V3" s="117"/>
+      <c r="W3" s="117"/>
+      <c r="X3" s="117"/>
+      <c r="Y3" s="117"/>
+      <c r="Z3" s="117"/>
+      <c r="AA3" s="117"/>
+      <c r="AB3" s="117"/>
+      <c r="AC3" s="117"/>
+      <c r="AD3" s="117"/>
+      <c r="AE3" s="117"/>
+      <c r="AF3" s="117"/>
+      <c r="AG3" s="117"/>
+      <c r="AH3" s="117"/>
+      <c r="AI3" s="117"/>
+      <c r="AJ3" s="117"/>
+      <c r="AK3" s="117"/>
+      <c r="AL3" s="117"/>
+      <c r="AM3" s="117"/>
+      <c r="AN3" s="117"/>
+      <c r="AO3" s="117"/>
+      <c r="AP3" s="117"/>
+      <c r="AQ3" s="117"/>
+      <c r="AR3" s="117"/>
+      <c r="AS3" s="117"/>
+      <c r="AT3" s="117"/>
+      <c r="AU3" s="117"/>
+      <c r="AV3" s="117"/>
     </row>
     <row r="4" spans="1:48" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="115"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="115"/>
-      <c r="S4" s="115"/>
-      <c r="T4" s="115"/>
-      <c r="U4" s="115"/>
-      <c r="V4" s="115"/>
-      <c r="W4" s="115"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="115"/>
-      <c r="Z4" s="115"/>
-      <c r="AA4" s="115"/>
-      <c r="AB4" s="115"/>
-      <c r="AC4" s="115"/>
-      <c r="AD4" s="115"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="115"/>
-      <c r="AG4" s="115"/>
-      <c r="AH4" s="115"/>
-      <c r="AI4" s="115"/>
-      <c r="AJ4" s="115"/>
-      <c r="AK4" s="115"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="115"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="115"/>
-      <c r="AP4" s="115"/>
-      <c r="AQ4" s="115"/>
-      <c r="AR4" s="115"/>
-      <c r="AS4" s="115"/>
-      <c r="AT4" s="115"/>
-      <c r="AU4" s="115"/>
-      <c r="AV4" s="115"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="117"/>
+      <c r="O4" s="117"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="117"/>
+      <c r="R4" s="117"/>
+      <c r="S4" s="117"/>
+      <c r="T4" s="117"/>
+      <c r="U4" s="117"/>
+      <c r="V4" s="117"/>
+      <c r="W4" s="117"/>
+      <c r="X4" s="117"/>
+      <c r="Y4" s="117"/>
+      <c r="Z4" s="117"/>
+      <c r="AA4" s="117"/>
+      <c r="AB4" s="117"/>
+      <c r="AC4" s="117"/>
+      <c r="AD4" s="117"/>
+      <c r="AE4" s="117"/>
+      <c r="AF4" s="117"/>
+      <c r="AG4" s="117"/>
+      <c r="AH4" s="117"/>
+      <c r="AI4" s="117"/>
+      <c r="AJ4" s="117"/>
+      <c r="AK4" s="117"/>
+      <c r="AL4" s="117"/>
+      <c r="AM4" s="117"/>
+      <c r="AN4" s="117"/>
+      <c r="AO4" s="117"/>
+      <c r="AP4" s="117"/>
+      <c r="AQ4" s="117"/>
+      <c r="AR4" s="117"/>
+      <c r="AS4" s="117"/>
+      <c r="AT4" s="117"/>
+      <c r="AU4" s="117"/>
+      <c r="AV4" s="117"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="115"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="115"/>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="115"/>
-      <c r="Y5" s="115"/>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
-      <c r="AD5" s="115"/>
-      <c r="AE5" s="115"/>
-      <c r="AF5" s="115"/>
-      <c r="AG5" s="115"/>
-      <c r="AH5" s="115"/>
-      <c r="AI5" s="115"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="115"/>
-      <c r="AM5" s="115"/>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
-      <c r="AS5" s="115"/>
-      <c r="AT5" s="115"/>
-      <c r="AU5" s="115"/>
-      <c r="AV5" s="115"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="117"/>
+      <c r="U5" s="117"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="117"/>
+      <c r="Z5" s="117"/>
+      <c r="AA5" s="117"/>
+      <c r="AB5" s="117"/>
+      <c r="AC5" s="117"/>
+      <c r="AD5" s="117"/>
+      <c r="AE5" s="117"/>
+      <c r="AF5" s="117"/>
+      <c r="AG5" s="117"/>
+      <c r="AH5" s="117"/>
+      <c r="AI5" s="117"/>
+      <c r="AJ5" s="117"/>
+      <c r="AK5" s="117"/>
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="117"/>
+      <c r="AN5" s="117"/>
+      <c r="AO5" s="117"/>
+      <c r="AP5" s="117"/>
+      <c r="AQ5" s="117"/>
+      <c r="AR5" s="117"/>
+      <c r="AS5" s="117"/>
+      <c r="AT5" s="117"/>
+      <c r="AU5" s="117"/>
+      <c r="AV5" s="117"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115"/>
-      <c r="W6" s="115"/>
-      <c r="X6" s="115"/>
-      <c r="Y6" s="115"/>
-      <c r="Z6" s="115"/>
-      <c r="AA6" s="115"/>
-      <c r="AB6" s="115"/>
-      <c r="AC6" s="115"/>
-      <c r="AD6" s="115"/>
-      <c r="AE6" s="115"/>
-      <c r="AF6" s="115"/>
-      <c r="AG6" s="115"/>
-      <c r="AH6" s="115"/>
-      <c r="AI6" s="115"/>
-      <c r="AJ6" s="115"/>
-      <c r="AK6" s="115"/>
-      <c r="AL6" s="115"/>
-      <c r="AM6" s="115"/>
-      <c r="AN6" s="115"/>
-      <c r="AO6" s="115"/>
-      <c r="AP6" s="115"/>
-      <c r="AQ6" s="115"/>
-      <c r="AR6" s="115"/>
-      <c r="AS6" s="115"/>
-      <c r="AT6" s="115"/>
-      <c r="AU6" s="115"/>
-      <c r="AV6" s="115"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="117"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="117"/>
+      <c r="R6" s="117"/>
+      <c r="S6" s="117"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="117"/>
+      <c r="V6" s="117"/>
+      <c r="W6" s="117"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="117"/>
+      <c r="AA6" s="117"/>
+      <c r="AB6" s="117"/>
+      <c r="AC6" s="117"/>
+      <c r="AD6" s="117"/>
+      <c r="AE6" s="117"/>
+      <c r="AF6" s="117"/>
+      <c r="AG6" s="117"/>
+      <c r="AH6" s="117"/>
+      <c r="AI6" s="117"/>
+      <c r="AJ6" s="117"/>
+      <c r="AK6" s="117"/>
+      <c r="AL6" s="117"/>
+      <c r="AM6" s="117"/>
+      <c r="AN6" s="117"/>
+      <c r="AO6" s="117"/>
+      <c r="AP6" s="117"/>
+      <c r="AQ6" s="117"/>
+      <c r="AR6" s="117"/>
+      <c r="AS6" s="117"/>
+      <c r="AT6" s="117"/>
+      <c r="AU6" s="117"/>
+      <c r="AV6" s="117"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="116" t="s">
+      <c r="B8" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="116" t="s">
+      <c r="D8" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="116" t="s">
+      <c r="E8" s="119" t="s">
         <v>272</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="119" t="s">
         <v>271</v>
       </c>
-      <c r="G8" s="116" t="s">
+      <c r="G8" s="119" t="s">
         <v>270</v>
       </c>
-      <c r="H8" s="116" t="s">
+      <c r="H8" s="119" t="s">
         <v>269</v>
       </c>
-      <c r="I8" s="116" t="s">
+      <c r="I8" s="119" t="s">
         <v>268</v>
       </c>
-      <c r="J8" s="116" t="s">
+      <c r="J8" s="119" t="s">
         <v>267</v>
       </c>
-      <c r="K8" s="116" t="s">
+      <c r="K8" s="119" t="s">
         <v>266</v>
       </c>
-      <c r="L8" s="116" t="s">
+      <c r="L8" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="M8" s="116" t="s">
+      <c r="M8" s="119" t="s">
         <v>264</v>
       </c>
-      <c r="N8" s="116" t="s">
+      <c r="N8" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="O8" s="116" t="s">
+      <c r="O8" s="119" t="s">
         <v>262</v>
       </c>
-      <c r="P8" s="116" t="s">
+      <c r="P8" s="119" t="s">
         <v>261</v>
       </c>
-      <c r="Q8" s="116" t="s">
+      <c r="Q8" s="119" t="s">
         <v>260</v>
       </c>
-      <c r="R8" s="116" t="s">
+      <c r="R8" s="119" t="s">
         <v>259</v>
       </c>
-      <c r="S8" s="116" t="s">
+      <c r="S8" s="119" t="s">
         <v>258</v>
       </c>
-      <c r="T8" s="116" t="s">
+      <c r="T8" s="119" t="s">
         <v>257</v>
       </c>
-      <c r="U8" s="116" t="s">
+      <c r="U8" s="119" t="s">
         <v>256</v>
       </c>
-      <c r="V8" s="116" t="s">
+      <c r="V8" s="119" t="s">
         <v>255</v>
       </c>
-      <c r="W8" s="116" t="s">
+      <c r="W8" s="119" t="s">
         <v>254</v>
       </c>
-      <c r="X8" s="116" t="s">
+      <c r="X8" s="119" t="s">
         <v>253</v>
       </c>
-      <c r="Y8" s="116" t="s">
+      <c r="Y8" s="119" t="s">
         <v>252</v>
       </c>
-      <c r="Z8" s="116" t="s">
+      <c r="Z8" s="119" t="s">
         <v>251</v>
       </c>
-      <c r="AA8" s="116" t="s">
+      <c r="AA8" s="119" t="s">
         <v>250</v>
       </c>
-      <c r="AB8" s="116" t="s">
+      <c r="AB8" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="AC8" s="116" t="s">
+      <c r="AC8" s="119" t="s">
         <v>248</v>
       </c>
-      <c r="AD8" s="116" t="s">
+      <c r="AD8" s="119" t="s">
         <v>247</v>
       </c>
-      <c r="AE8" s="116" t="s">
+      <c r="AE8" s="119" t="s">
         <v>246</v>
       </c>
-      <c r="AF8" s="116" t="s">
+      <c r="AF8" s="119" t="s">
         <v>245</v>
       </c>
-      <c r="AG8" s="116" t="s">
+      <c r="AG8" s="119" t="s">
         <v>244</v>
       </c>
-      <c r="AH8" s="116" t="s">
+      <c r="AH8" s="119" t="s">
         <v>243</v>
       </c>
-      <c r="AI8" s="116" t="s">
+      <c r="AI8" s="119" t="s">
         <v>242</v>
       </c>
-      <c r="AJ8" s="116" t="s">
+      <c r="AJ8" s="119" t="s">
         <v>241</v>
       </c>
-      <c r="AK8" s="116" t="s">
+      <c r="AK8" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="AL8" s="116" t="s">
+      <c r="AL8" s="119" t="s">
         <v>239</v>
       </c>
-      <c r="AM8" s="116" t="s">
+      <c r="AM8" s="119" t="s">
         <v>238</v>
       </c>
-      <c r="AN8" s="116" t="s">
+      <c r="AN8" s="119" t="s">
         <v>237</v>
       </c>
-      <c r="AO8" s="116" t="s">
+      <c r="AO8" s="119" t="s">
         <v>236</v>
       </c>
-      <c r="AP8" s="116" t="s">
+      <c r="AP8" s="119" t="s">
         <v>235</v>
       </c>
-      <c r="AQ8" s="116" t="s">
+      <c r="AQ8" s="119" t="s">
         <v>234</v>
       </c>
-      <c r="AR8" s="116" t="s">
+      <c r="AR8" s="119" t="s">
         <v>233</v>
       </c>
-      <c r="AS8" s="116" t="s">
+      <c r="AS8" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="AT8" s="116" t="s">
+      <c r="AT8" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="AU8" s="116" t="s">
+      <c r="AU8" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="AV8" s="116" t="s">
+      <c r="AV8" s="119" t="s">
         <v>35</v>
       </c>
     </row>
@@ -25609,475 +25609,520 @@
       </c>
     </row>
     <row r="105" spans="1:48" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A105" s="117" t="s">
+      <c r="A105" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="B105" s="115"/>
-      <c r="C105" s="115"/>
-      <c r="D105" s="115"/>
-      <c r="E105" s="115"/>
-      <c r="F105" s="115"/>
-      <c r="G105" s="115"/>
-      <c r="H105" s="115"/>
-      <c r="I105" s="115"/>
-      <c r="J105" s="115"/>
-      <c r="K105" s="115"/>
-      <c r="L105" s="115"/>
-      <c r="M105" s="115"/>
-      <c r="N105" s="115"/>
-      <c r="O105" s="115"/>
-      <c r="P105" s="115"/>
-      <c r="Q105" s="115"/>
-      <c r="R105" s="115"/>
-      <c r="S105" s="115"/>
-      <c r="T105" s="115"/>
-      <c r="U105" s="115"/>
-      <c r="V105" s="115"/>
-      <c r="W105" s="115"/>
-      <c r="X105" s="115"/>
-      <c r="Y105" s="115"/>
-      <c r="Z105" s="115"/>
-      <c r="AA105" s="115"/>
-      <c r="AB105" s="115"/>
-      <c r="AC105" s="115"/>
-      <c r="AD105" s="115"/>
-      <c r="AE105" s="115"/>
-      <c r="AF105" s="115"/>
-      <c r="AG105" s="115"/>
-      <c r="AH105" s="115"/>
-      <c r="AI105" s="115"/>
-      <c r="AJ105" s="115"/>
-      <c r="AK105" s="115"/>
-      <c r="AL105" s="115"/>
-      <c r="AM105" s="115"/>
-      <c r="AN105" s="115"/>
-      <c r="AO105" s="115"/>
-      <c r="AP105" s="115"/>
-      <c r="AQ105" s="115"/>
-      <c r="AR105" s="115"/>
-      <c r="AS105" s="115"/>
-      <c r="AT105" s="115"/>
-      <c r="AU105" s="115"/>
-      <c r="AV105" s="115"/>
+      <c r="B105" s="117"/>
+      <c r="C105" s="117"/>
+      <c r="D105" s="117"/>
+      <c r="E105" s="117"/>
+      <c r="F105" s="117"/>
+      <c r="G105" s="117"/>
+      <c r="H105" s="117"/>
+      <c r="I105" s="117"/>
+      <c r="J105" s="117"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="117"/>
+      <c r="M105" s="117"/>
+      <c r="N105" s="117"/>
+      <c r="O105" s="117"/>
+      <c r="P105" s="117"/>
+      <c r="Q105" s="117"/>
+      <c r="R105" s="117"/>
+      <c r="S105" s="117"/>
+      <c r="T105" s="117"/>
+      <c r="U105" s="117"/>
+      <c r="V105" s="117"/>
+      <c r="W105" s="117"/>
+      <c r="X105" s="117"/>
+      <c r="Y105" s="117"/>
+      <c r="Z105" s="117"/>
+      <c r="AA105" s="117"/>
+      <c r="AB105" s="117"/>
+      <c r="AC105" s="117"/>
+      <c r="AD105" s="117"/>
+      <c r="AE105" s="117"/>
+      <c r="AF105" s="117"/>
+      <c r="AG105" s="117"/>
+      <c r="AH105" s="117"/>
+      <c r="AI105" s="117"/>
+      <c r="AJ105" s="117"/>
+      <c r="AK105" s="117"/>
+      <c r="AL105" s="117"/>
+      <c r="AM105" s="117"/>
+      <c r="AN105" s="117"/>
+      <c r="AO105" s="117"/>
+      <c r="AP105" s="117"/>
+      <c r="AQ105" s="117"/>
+      <c r="AR105" s="117"/>
+      <c r="AS105" s="117"/>
+      <c r="AT105" s="117"/>
+      <c r="AU105" s="117"/>
+      <c r="AV105" s="117"/>
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A106" s="114" t="s">
+      <c r="A106" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="B106" s="115"/>
-      <c r="C106" s="115"/>
-      <c r="D106" s="115"/>
-      <c r="E106" s="115"/>
-      <c r="F106" s="115"/>
-      <c r="G106" s="115"/>
-      <c r="H106" s="115"/>
-      <c r="I106" s="115"/>
-      <c r="J106" s="115"/>
-      <c r="K106" s="115"/>
-      <c r="L106" s="115"/>
-      <c r="M106" s="115"/>
-      <c r="N106" s="115"/>
-      <c r="O106" s="115"/>
-      <c r="P106" s="115"/>
-      <c r="Q106" s="115"/>
-      <c r="R106" s="115"/>
-      <c r="S106" s="115"/>
-      <c r="T106" s="115"/>
-      <c r="U106" s="115"/>
-      <c r="V106" s="115"/>
-      <c r="W106" s="115"/>
-      <c r="X106" s="115"/>
-      <c r="Y106" s="115"/>
-      <c r="Z106" s="115"/>
-      <c r="AA106" s="115"/>
-      <c r="AB106" s="115"/>
-      <c r="AC106" s="115"/>
-      <c r="AD106" s="115"/>
-      <c r="AE106" s="115"/>
-      <c r="AF106" s="115"/>
-      <c r="AG106" s="115"/>
-      <c r="AH106" s="115"/>
-      <c r="AI106" s="115"/>
-      <c r="AJ106" s="115"/>
-      <c r="AK106" s="115"/>
-      <c r="AL106" s="115"/>
-      <c r="AM106" s="115"/>
-      <c r="AN106" s="115"/>
-      <c r="AO106" s="115"/>
-      <c r="AP106" s="115"/>
-      <c r="AQ106" s="115"/>
-      <c r="AR106" s="115"/>
-      <c r="AS106" s="115"/>
-      <c r="AT106" s="115"/>
-      <c r="AU106" s="115"/>
-      <c r="AV106" s="115"/>
+      <c r="B106" s="117"/>
+      <c r="C106" s="117"/>
+      <c r="D106" s="117"/>
+      <c r="E106" s="117"/>
+      <c r="F106" s="117"/>
+      <c r="G106" s="117"/>
+      <c r="H106" s="117"/>
+      <c r="I106" s="117"/>
+      <c r="J106" s="117"/>
+      <c r="K106" s="117"/>
+      <c r="L106" s="117"/>
+      <c r="M106" s="117"/>
+      <c r="N106" s="117"/>
+      <c r="O106" s="117"/>
+      <c r="P106" s="117"/>
+      <c r="Q106" s="117"/>
+      <c r="R106" s="117"/>
+      <c r="S106" s="117"/>
+      <c r="T106" s="117"/>
+      <c r="U106" s="117"/>
+      <c r="V106" s="117"/>
+      <c r="W106" s="117"/>
+      <c r="X106" s="117"/>
+      <c r="Y106" s="117"/>
+      <c r="Z106" s="117"/>
+      <c r="AA106" s="117"/>
+      <c r="AB106" s="117"/>
+      <c r="AC106" s="117"/>
+      <c r="AD106" s="117"/>
+      <c r="AE106" s="117"/>
+      <c r="AF106" s="117"/>
+      <c r="AG106" s="117"/>
+      <c r="AH106" s="117"/>
+      <c r="AI106" s="117"/>
+      <c r="AJ106" s="117"/>
+      <c r="AK106" s="117"/>
+      <c r="AL106" s="117"/>
+      <c r="AM106" s="117"/>
+      <c r="AN106" s="117"/>
+      <c r="AO106" s="117"/>
+      <c r="AP106" s="117"/>
+      <c r="AQ106" s="117"/>
+      <c r="AR106" s="117"/>
+      <c r="AS106" s="117"/>
+      <c r="AT106" s="117"/>
+      <c r="AU106" s="117"/>
+      <c r="AV106" s="117"/>
     </row>
     <row r="107" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A107" s="114" t="s">
+      <c r="A107" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="B107" s="115"/>
-      <c r="C107" s="115"/>
-      <c r="D107" s="115"/>
-      <c r="E107" s="115"/>
-      <c r="F107" s="115"/>
-      <c r="G107" s="115"/>
-      <c r="H107" s="115"/>
-      <c r="I107" s="115"/>
-      <c r="J107" s="115"/>
-      <c r="K107" s="115"/>
-      <c r="L107" s="115"/>
-      <c r="M107" s="115"/>
-      <c r="N107" s="115"/>
-      <c r="O107" s="115"/>
-      <c r="P107" s="115"/>
-      <c r="Q107" s="115"/>
-      <c r="R107" s="115"/>
-      <c r="S107" s="115"/>
-      <c r="T107" s="115"/>
-      <c r="U107" s="115"/>
-      <c r="V107" s="115"/>
-      <c r="W107" s="115"/>
-      <c r="X107" s="115"/>
-      <c r="Y107" s="115"/>
-      <c r="Z107" s="115"/>
-      <c r="AA107" s="115"/>
-      <c r="AB107" s="115"/>
-      <c r="AC107" s="115"/>
-      <c r="AD107" s="115"/>
-      <c r="AE107" s="115"/>
-      <c r="AF107" s="115"/>
-      <c r="AG107" s="115"/>
-      <c r="AH107" s="115"/>
-      <c r="AI107" s="115"/>
-      <c r="AJ107" s="115"/>
-      <c r="AK107" s="115"/>
-      <c r="AL107" s="115"/>
-      <c r="AM107" s="115"/>
-      <c r="AN107" s="115"/>
-      <c r="AO107" s="115"/>
-      <c r="AP107" s="115"/>
-      <c r="AQ107" s="115"/>
-      <c r="AR107" s="115"/>
-      <c r="AS107" s="115"/>
-      <c r="AT107" s="115"/>
-      <c r="AU107" s="115"/>
-      <c r="AV107" s="115"/>
+      <c r="B107" s="117"/>
+      <c r="C107" s="117"/>
+      <c r="D107" s="117"/>
+      <c r="E107" s="117"/>
+      <c r="F107" s="117"/>
+      <c r="G107" s="117"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="117"/>
+      <c r="J107" s="117"/>
+      <c r="K107" s="117"/>
+      <c r="L107" s="117"/>
+      <c r="M107" s="117"/>
+      <c r="N107" s="117"/>
+      <c r="O107" s="117"/>
+      <c r="P107" s="117"/>
+      <c r="Q107" s="117"/>
+      <c r="R107" s="117"/>
+      <c r="S107" s="117"/>
+      <c r="T107" s="117"/>
+      <c r="U107" s="117"/>
+      <c r="V107" s="117"/>
+      <c r="W107" s="117"/>
+      <c r="X107" s="117"/>
+      <c r="Y107" s="117"/>
+      <c r="Z107" s="117"/>
+      <c r="AA107" s="117"/>
+      <c r="AB107" s="117"/>
+      <c r="AC107" s="117"/>
+      <c r="AD107" s="117"/>
+      <c r="AE107" s="117"/>
+      <c r="AF107" s="117"/>
+      <c r="AG107" s="117"/>
+      <c r="AH107" s="117"/>
+      <c r="AI107" s="117"/>
+      <c r="AJ107" s="117"/>
+      <c r="AK107" s="117"/>
+      <c r="AL107" s="117"/>
+      <c r="AM107" s="117"/>
+      <c r="AN107" s="117"/>
+      <c r="AO107" s="117"/>
+      <c r="AP107" s="117"/>
+      <c r="AQ107" s="117"/>
+      <c r="AR107" s="117"/>
+      <c r="AS107" s="117"/>
+      <c r="AT107" s="117"/>
+      <c r="AU107" s="117"/>
+      <c r="AV107" s="117"/>
     </row>
     <row r="108" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A108" s="114" t="s">
+      <c r="A108" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="B108" s="115"/>
-      <c r="C108" s="115"/>
-      <c r="D108" s="115"/>
-      <c r="E108" s="115"/>
-      <c r="F108" s="115"/>
-      <c r="G108" s="115"/>
-      <c r="H108" s="115"/>
-      <c r="I108" s="115"/>
-      <c r="J108" s="115"/>
-      <c r="K108" s="115"/>
-      <c r="L108" s="115"/>
-      <c r="M108" s="115"/>
-      <c r="N108" s="115"/>
-      <c r="O108" s="115"/>
-      <c r="P108" s="115"/>
-      <c r="Q108" s="115"/>
-      <c r="R108" s="115"/>
-      <c r="S108" s="115"/>
-      <c r="T108" s="115"/>
-      <c r="U108" s="115"/>
-      <c r="V108" s="115"/>
-      <c r="W108" s="115"/>
-      <c r="X108" s="115"/>
-      <c r="Y108" s="115"/>
-      <c r="Z108" s="115"/>
-      <c r="AA108" s="115"/>
-      <c r="AB108" s="115"/>
-      <c r="AC108" s="115"/>
-      <c r="AD108" s="115"/>
-      <c r="AE108" s="115"/>
-      <c r="AF108" s="115"/>
-      <c r="AG108" s="115"/>
-      <c r="AH108" s="115"/>
-      <c r="AI108" s="115"/>
-      <c r="AJ108" s="115"/>
-      <c r="AK108" s="115"/>
-      <c r="AL108" s="115"/>
-      <c r="AM108" s="115"/>
-      <c r="AN108" s="115"/>
-      <c r="AO108" s="115"/>
-      <c r="AP108" s="115"/>
-      <c r="AQ108" s="115"/>
-      <c r="AR108" s="115"/>
-      <c r="AS108" s="115"/>
-      <c r="AT108" s="115"/>
-      <c r="AU108" s="115"/>
-      <c r="AV108" s="115"/>
+      <c r="B108" s="117"/>
+      <c r="C108" s="117"/>
+      <c r="D108" s="117"/>
+      <c r="E108" s="117"/>
+      <c r="F108" s="117"/>
+      <c r="G108" s="117"/>
+      <c r="H108" s="117"/>
+      <c r="I108" s="117"/>
+      <c r="J108" s="117"/>
+      <c r="K108" s="117"/>
+      <c r="L108" s="117"/>
+      <c r="M108" s="117"/>
+      <c r="N108" s="117"/>
+      <c r="O108" s="117"/>
+      <c r="P108" s="117"/>
+      <c r="Q108" s="117"/>
+      <c r="R108" s="117"/>
+      <c r="S108" s="117"/>
+      <c r="T108" s="117"/>
+      <c r="U108" s="117"/>
+      <c r="V108" s="117"/>
+      <c r="W108" s="117"/>
+      <c r="X108" s="117"/>
+      <c r="Y108" s="117"/>
+      <c r="Z108" s="117"/>
+      <c r="AA108" s="117"/>
+      <c r="AB108" s="117"/>
+      <c r="AC108" s="117"/>
+      <c r="AD108" s="117"/>
+      <c r="AE108" s="117"/>
+      <c r="AF108" s="117"/>
+      <c r="AG108" s="117"/>
+      <c r="AH108" s="117"/>
+      <c r="AI108" s="117"/>
+      <c r="AJ108" s="117"/>
+      <c r="AK108" s="117"/>
+      <c r="AL108" s="117"/>
+      <c r="AM108" s="117"/>
+      <c r="AN108" s="117"/>
+      <c r="AO108" s="117"/>
+      <c r="AP108" s="117"/>
+      <c r="AQ108" s="117"/>
+      <c r="AR108" s="117"/>
+      <c r="AS108" s="117"/>
+      <c r="AT108" s="117"/>
+      <c r="AU108" s="117"/>
+      <c r="AV108" s="117"/>
     </row>
     <row r="109" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A109" s="114" t="s">
+      <c r="A109" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="B109" s="115"/>
-      <c r="C109" s="115"/>
-      <c r="D109" s="115"/>
-      <c r="E109" s="115"/>
-      <c r="F109" s="115"/>
-      <c r="G109" s="115"/>
-      <c r="H109" s="115"/>
-      <c r="I109" s="115"/>
-      <c r="J109" s="115"/>
-      <c r="K109" s="115"/>
-      <c r="L109" s="115"/>
-      <c r="M109" s="115"/>
-      <c r="N109" s="115"/>
-      <c r="O109" s="115"/>
-      <c r="P109" s="115"/>
-      <c r="Q109" s="115"/>
-      <c r="R109" s="115"/>
-      <c r="S109" s="115"/>
-      <c r="T109" s="115"/>
-      <c r="U109" s="115"/>
-      <c r="V109" s="115"/>
-      <c r="W109" s="115"/>
-      <c r="X109" s="115"/>
-      <c r="Y109" s="115"/>
-      <c r="Z109" s="115"/>
-      <c r="AA109" s="115"/>
-      <c r="AB109" s="115"/>
-      <c r="AC109" s="115"/>
-      <c r="AD109" s="115"/>
-      <c r="AE109" s="115"/>
-      <c r="AF109" s="115"/>
-      <c r="AG109" s="115"/>
-      <c r="AH109" s="115"/>
-      <c r="AI109" s="115"/>
-      <c r="AJ109" s="115"/>
-      <c r="AK109" s="115"/>
-      <c r="AL109" s="115"/>
-      <c r="AM109" s="115"/>
-      <c r="AN109" s="115"/>
-      <c r="AO109" s="115"/>
-      <c r="AP109" s="115"/>
-      <c r="AQ109" s="115"/>
-      <c r="AR109" s="115"/>
-      <c r="AS109" s="115"/>
-      <c r="AT109" s="115"/>
-      <c r="AU109" s="115"/>
-      <c r="AV109" s="115"/>
+      <c r="B109" s="117"/>
+      <c r="C109" s="117"/>
+      <c r="D109" s="117"/>
+      <c r="E109" s="117"/>
+      <c r="F109" s="117"/>
+      <c r="G109" s="117"/>
+      <c r="H109" s="117"/>
+      <c r="I109" s="117"/>
+      <c r="J109" s="117"/>
+      <c r="K109" s="117"/>
+      <c r="L109" s="117"/>
+      <c r="M109" s="117"/>
+      <c r="N109" s="117"/>
+      <c r="O109" s="117"/>
+      <c r="P109" s="117"/>
+      <c r="Q109" s="117"/>
+      <c r="R109" s="117"/>
+      <c r="S109" s="117"/>
+      <c r="T109" s="117"/>
+      <c r="U109" s="117"/>
+      <c r="V109" s="117"/>
+      <c r="W109" s="117"/>
+      <c r="X109" s="117"/>
+      <c r="Y109" s="117"/>
+      <c r="Z109" s="117"/>
+      <c r="AA109" s="117"/>
+      <c r="AB109" s="117"/>
+      <c r="AC109" s="117"/>
+      <c r="AD109" s="117"/>
+      <c r="AE109" s="117"/>
+      <c r="AF109" s="117"/>
+      <c r="AG109" s="117"/>
+      <c r="AH109" s="117"/>
+      <c r="AI109" s="117"/>
+      <c r="AJ109" s="117"/>
+      <c r="AK109" s="117"/>
+      <c r="AL109" s="117"/>
+      <c r="AM109" s="117"/>
+      <c r="AN109" s="117"/>
+      <c r="AO109" s="117"/>
+      <c r="AP109" s="117"/>
+      <c r="AQ109" s="117"/>
+      <c r="AR109" s="117"/>
+      <c r="AS109" s="117"/>
+      <c r="AT109" s="117"/>
+      <c r="AU109" s="117"/>
+      <c r="AV109" s="117"/>
     </row>
     <row r="110" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A110" s="114" t="s">
+      <c r="A110" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="B110" s="115"/>
-      <c r="C110" s="115"/>
-      <c r="D110" s="115"/>
-      <c r="E110" s="115"/>
-      <c r="F110" s="115"/>
-      <c r="G110" s="115"/>
-      <c r="H110" s="115"/>
-      <c r="I110" s="115"/>
-      <c r="J110" s="115"/>
-      <c r="K110" s="115"/>
-      <c r="L110" s="115"/>
-      <c r="M110" s="115"/>
-      <c r="N110" s="115"/>
-      <c r="O110" s="115"/>
-      <c r="P110" s="115"/>
-      <c r="Q110" s="115"/>
-      <c r="R110" s="115"/>
-      <c r="S110" s="115"/>
-      <c r="T110" s="115"/>
-      <c r="U110" s="115"/>
-      <c r="V110" s="115"/>
-      <c r="W110" s="115"/>
-      <c r="X110" s="115"/>
-      <c r="Y110" s="115"/>
-      <c r="Z110" s="115"/>
-      <c r="AA110" s="115"/>
-      <c r="AB110" s="115"/>
-      <c r="AC110" s="115"/>
-      <c r="AD110" s="115"/>
-      <c r="AE110" s="115"/>
-      <c r="AF110" s="115"/>
-      <c r="AG110" s="115"/>
-      <c r="AH110" s="115"/>
-      <c r="AI110" s="115"/>
-      <c r="AJ110" s="115"/>
-      <c r="AK110" s="115"/>
-      <c r="AL110" s="115"/>
-      <c r="AM110" s="115"/>
-      <c r="AN110" s="115"/>
-      <c r="AO110" s="115"/>
-      <c r="AP110" s="115"/>
-      <c r="AQ110" s="115"/>
-      <c r="AR110" s="115"/>
-      <c r="AS110" s="115"/>
-      <c r="AT110" s="115"/>
-      <c r="AU110" s="115"/>
-      <c r="AV110" s="115"/>
+      <c r="B110" s="117"/>
+      <c r="C110" s="117"/>
+      <c r="D110" s="117"/>
+      <c r="E110" s="117"/>
+      <c r="F110" s="117"/>
+      <c r="G110" s="117"/>
+      <c r="H110" s="117"/>
+      <c r="I110" s="117"/>
+      <c r="J110" s="117"/>
+      <c r="K110" s="117"/>
+      <c r="L110" s="117"/>
+      <c r="M110" s="117"/>
+      <c r="N110" s="117"/>
+      <c r="O110" s="117"/>
+      <c r="P110" s="117"/>
+      <c r="Q110" s="117"/>
+      <c r="R110" s="117"/>
+      <c r="S110" s="117"/>
+      <c r="T110" s="117"/>
+      <c r="U110" s="117"/>
+      <c r="V110" s="117"/>
+      <c r="W110" s="117"/>
+      <c r="X110" s="117"/>
+      <c r="Y110" s="117"/>
+      <c r="Z110" s="117"/>
+      <c r="AA110" s="117"/>
+      <c r="AB110" s="117"/>
+      <c r="AC110" s="117"/>
+      <c r="AD110" s="117"/>
+      <c r="AE110" s="117"/>
+      <c r="AF110" s="117"/>
+      <c r="AG110" s="117"/>
+      <c r="AH110" s="117"/>
+      <c r="AI110" s="117"/>
+      <c r="AJ110" s="117"/>
+      <c r="AK110" s="117"/>
+      <c r="AL110" s="117"/>
+      <c r="AM110" s="117"/>
+      <c r="AN110" s="117"/>
+      <c r="AO110" s="117"/>
+      <c r="AP110" s="117"/>
+      <c r="AQ110" s="117"/>
+      <c r="AR110" s="117"/>
+      <c r="AS110" s="117"/>
+      <c r="AT110" s="117"/>
+      <c r="AU110" s="117"/>
+      <c r="AV110" s="117"/>
     </row>
     <row r="111" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A111" s="114" t="s">
+      <c r="A111" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="B111" s="115"/>
-      <c r="C111" s="115"/>
-      <c r="D111" s="115"/>
-      <c r="E111" s="115"/>
-      <c r="F111" s="115"/>
-      <c r="G111" s="115"/>
-      <c r="H111" s="115"/>
-      <c r="I111" s="115"/>
-      <c r="J111" s="115"/>
-      <c r="K111" s="115"/>
-      <c r="L111" s="115"/>
-      <c r="M111" s="115"/>
-      <c r="N111" s="115"/>
-      <c r="O111" s="115"/>
-      <c r="P111" s="115"/>
-      <c r="Q111" s="115"/>
-      <c r="R111" s="115"/>
-      <c r="S111" s="115"/>
-      <c r="T111" s="115"/>
-      <c r="U111" s="115"/>
-      <c r="V111" s="115"/>
-      <c r="W111" s="115"/>
-      <c r="X111" s="115"/>
-      <c r="Y111" s="115"/>
-      <c r="Z111" s="115"/>
-      <c r="AA111" s="115"/>
-      <c r="AB111" s="115"/>
-      <c r="AC111" s="115"/>
-      <c r="AD111" s="115"/>
-      <c r="AE111" s="115"/>
-      <c r="AF111" s="115"/>
-      <c r="AG111" s="115"/>
-      <c r="AH111" s="115"/>
-      <c r="AI111" s="115"/>
-      <c r="AJ111" s="115"/>
-      <c r="AK111" s="115"/>
-      <c r="AL111" s="115"/>
-      <c r="AM111" s="115"/>
-      <c r="AN111" s="115"/>
-      <c r="AO111" s="115"/>
-      <c r="AP111" s="115"/>
-      <c r="AQ111" s="115"/>
-      <c r="AR111" s="115"/>
-      <c r="AS111" s="115"/>
-      <c r="AT111" s="115"/>
-      <c r="AU111" s="115"/>
-      <c r="AV111" s="115"/>
+      <c r="B111" s="117"/>
+      <c r="C111" s="117"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="117"/>
+      <c r="F111" s="117"/>
+      <c r="G111" s="117"/>
+      <c r="H111" s="117"/>
+      <c r="I111" s="117"/>
+      <c r="J111" s="117"/>
+      <c r="K111" s="117"/>
+      <c r="L111" s="117"/>
+      <c r="M111" s="117"/>
+      <c r="N111" s="117"/>
+      <c r="O111" s="117"/>
+      <c r="P111" s="117"/>
+      <c r="Q111" s="117"/>
+      <c r="R111" s="117"/>
+      <c r="S111" s="117"/>
+      <c r="T111" s="117"/>
+      <c r="U111" s="117"/>
+      <c r="V111" s="117"/>
+      <c r="W111" s="117"/>
+      <c r="X111" s="117"/>
+      <c r="Y111" s="117"/>
+      <c r="Z111" s="117"/>
+      <c r="AA111" s="117"/>
+      <c r="AB111" s="117"/>
+      <c r="AC111" s="117"/>
+      <c r="AD111" s="117"/>
+      <c r="AE111" s="117"/>
+      <c r="AF111" s="117"/>
+      <c r="AG111" s="117"/>
+      <c r="AH111" s="117"/>
+      <c r="AI111" s="117"/>
+      <c r="AJ111" s="117"/>
+      <c r="AK111" s="117"/>
+      <c r="AL111" s="117"/>
+      <c r="AM111" s="117"/>
+      <c r="AN111" s="117"/>
+      <c r="AO111" s="117"/>
+      <c r="AP111" s="117"/>
+      <c r="AQ111" s="117"/>
+      <c r="AR111" s="117"/>
+      <c r="AS111" s="117"/>
+      <c r="AT111" s="117"/>
+      <c r="AU111" s="117"/>
+      <c r="AV111" s="117"/>
     </row>
     <row r="112" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A112" s="114" t="s">
+      <c r="A112" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="B112" s="115"/>
-      <c r="C112" s="115"/>
-      <c r="D112" s="115"/>
-      <c r="E112" s="115"/>
-      <c r="F112" s="115"/>
-      <c r="G112" s="115"/>
-      <c r="H112" s="115"/>
-      <c r="I112" s="115"/>
-      <c r="J112" s="115"/>
-      <c r="K112" s="115"/>
-      <c r="L112" s="115"/>
-      <c r="M112" s="115"/>
-      <c r="N112" s="115"/>
-      <c r="O112" s="115"/>
-      <c r="P112" s="115"/>
-      <c r="Q112" s="115"/>
-      <c r="R112" s="115"/>
-      <c r="S112" s="115"/>
-      <c r="T112" s="115"/>
-      <c r="U112" s="115"/>
-      <c r="V112" s="115"/>
-      <c r="W112" s="115"/>
-      <c r="X112" s="115"/>
-      <c r="Y112" s="115"/>
-      <c r="Z112" s="115"/>
-      <c r="AA112" s="115"/>
-      <c r="AB112" s="115"/>
-      <c r="AC112" s="115"/>
-      <c r="AD112" s="115"/>
-      <c r="AE112" s="115"/>
-      <c r="AF112" s="115"/>
-      <c r="AG112" s="115"/>
-      <c r="AH112" s="115"/>
-      <c r="AI112" s="115"/>
-      <c r="AJ112" s="115"/>
-      <c r="AK112" s="115"/>
-      <c r="AL112" s="115"/>
-      <c r="AM112" s="115"/>
-      <c r="AN112" s="115"/>
-      <c r="AO112" s="115"/>
-      <c r="AP112" s="115"/>
-      <c r="AQ112" s="115"/>
-      <c r="AR112" s="115"/>
-      <c r="AS112" s="115"/>
-      <c r="AT112" s="115"/>
-      <c r="AU112" s="115"/>
-      <c r="AV112" s="115"/>
+      <c r="B112" s="117"/>
+      <c r="C112" s="117"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="117"/>
+      <c r="F112" s="117"/>
+      <c r="G112" s="117"/>
+      <c r="H112" s="117"/>
+      <c r="I112" s="117"/>
+      <c r="J112" s="117"/>
+      <c r="K112" s="117"/>
+      <c r="L112" s="117"/>
+      <c r="M112" s="117"/>
+      <c r="N112" s="117"/>
+      <c r="O112" s="117"/>
+      <c r="P112" s="117"/>
+      <c r="Q112" s="117"/>
+      <c r="R112" s="117"/>
+      <c r="S112" s="117"/>
+      <c r="T112" s="117"/>
+      <c r="U112" s="117"/>
+      <c r="V112" s="117"/>
+      <c r="W112" s="117"/>
+      <c r="X112" s="117"/>
+      <c r="Y112" s="117"/>
+      <c r="Z112" s="117"/>
+      <c r="AA112" s="117"/>
+      <c r="AB112" s="117"/>
+      <c r="AC112" s="117"/>
+      <c r="AD112" s="117"/>
+      <c r="AE112" s="117"/>
+      <c r="AF112" s="117"/>
+      <c r="AG112" s="117"/>
+      <c r="AH112" s="117"/>
+      <c r="AI112" s="117"/>
+      <c r="AJ112" s="117"/>
+      <c r="AK112" s="117"/>
+      <c r="AL112" s="117"/>
+      <c r="AM112" s="117"/>
+      <c r="AN112" s="117"/>
+      <c r="AO112" s="117"/>
+      <c r="AP112" s="117"/>
+      <c r="AQ112" s="117"/>
+      <c r="AR112" s="117"/>
+      <c r="AS112" s="117"/>
+      <c r="AT112" s="117"/>
+      <c r="AU112" s="117"/>
+      <c r="AV112" s="117"/>
     </row>
     <row r="113" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A113" s="114" t="s">
+      <c r="A113" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="B113" s="115"/>
-      <c r="C113" s="115"/>
-      <c r="D113" s="115"/>
-      <c r="E113" s="115"/>
-      <c r="F113" s="115"/>
-      <c r="G113" s="115"/>
-      <c r="H113" s="115"/>
-      <c r="I113" s="115"/>
-      <c r="J113" s="115"/>
-      <c r="K113" s="115"/>
-      <c r="L113" s="115"/>
-      <c r="M113" s="115"/>
-      <c r="N113" s="115"/>
-      <c r="O113" s="115"/>
-      <c r="P113" s="115"/>
-      <c r="Q113" s="115"/>
-      <c r="R113" s="115"/>
-      <c r="S113" s="115"/>
-      <c r="T113" s="115"/>
-      <c r="U113" s="115"/>
-      <c r="V113" s="115"/>
-      <c r="W113" s="115"/>
-      <c r="X113" s="115"/>
-      <c r="Y113" s="115"/>
-      <c r="Z113" s="115"/>
-      <c r="AA113" s="115"/>
-      <c r="AB113" s="115"/>
-      <c r="AC113" s="115"/>
-      <c r="AD113" s="115"/>
-      <c r="AE113" s="115"/>
-      <c r="AF113" s="115"/>
-      <c r="AG113" s="115"/>
-      <c r="AH113" s="115"/>
-      <c r="AI113" s="115"/>
-      <c r="AJ113" s="115"/>
-      <c r="AK113" s="115"/>
-      <c r="AL113" s="115"/>
-      <c r="AM113" s="115"/>
-      <c r="AN113" s="115"/>
-      <c r="AO113" s="115"/>
-      <c r="AP113" s="115"/>
-      <c r="AQ113" s="115"/>
-      <c r="AR113" s="115"/>
-      <c r="AS113" s="115"/>
-      <c r="AT113" s="115"/>
-      <c r="AU113" s="115"/>
-      <c r="AV113" s="115"/>
+      <c r="B113" s="117"/>
+      <c r="C113" s="117"/>
+      <c r="D113" s="117"/>
+      <c r="E113" s="117"/>
+      <c r="F113" s="117"/>
+      <c r="G113" s="117"/>
+      <c r="H113" s="117"/>
+      <c r="I113" s="117"/>
+      <c r="J113" s="117"/>
+      <c r="K113" s="117"/>
+      <c r="L113" s="117"/>
+      <c r="M113" s="117"/>
+      <c r="N113" s="117"/>
+      <c r="O113" s="117"/>
+      <c r="P113" s="117"/>
+      <c r="Q113" s="117"/>
+      <c r="R113" s="117"/>
+      <c r="S113" s="117"/>
+      <c r="T113" s="117"/>
+      <c r="U113" s="117"/>
+      <c r="V113" s="117"/>
+      <c r="W113" s="117"/>
+      <c r="X113" s="117"/>
+      <c r="Y113" s="117"/>
+      <c r="Z113" s="117"/>
+      <c r="AA113" s="117"/>
+      <c r="AB113" s="117"/>
+      <c r="AC113" s="117"/>
+      <c r="AD113" s="117"/>
+      <c r="AE113" s="117"/>
+      <c r="AF113" s="117"/>
+      <c r="AG113" s="117"/>
+      <c r="AH113" s="117"/>
+      <c r="AI113" s="117"/>
+      <c r="AJ113" s="117"/>
+      <c r="AK113" s="117"/>
+      <c r="AL113" s="117"/>
+      <c r="AM113" s="117"/>
+      <c r="AN113" s="117"/>
+      <c r="AO113" s="117"/>
+      <c r="AP113" s="117"/>
+      <c r="AQ113" s="117"/>
+      <c r="AR113" s="117"/>
+      <c r="AS113" s="117"/>
+      <c r="AT113" s="117"/>
+      <c r="AU113" s="117"/>
+      <c r="AV113" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="AV8"/>
+    <mergeCell ref="A111:AV111"/>
+    <mergeCell ref="A112:AV112"/>
+    <mergeCell ref="A113:AV113"/>
+    <mergeCell ref="A105:AV105"/>
+    <mergeCell ref="A106:AV106"/>
+    <mergeCell ref="A107:AV107"/>
+    <mergeCell ref="A108:AV108"/>
+    <mergeCell ref="A109:AV109"/>
+    <mergeCell ref="A110:AV110"/>
+    <mergeCell ref="AQ8"/>
+    <mergeCell ref="AR8"/>
+    <mergeCell ref="AS8"/>
+    <mergeCell ref="AT8"/>
+    <mergeCell ref="AU8"/>
+    <mergeCell ref="AL8"/>
+    <mergeCell ref="AM8"/>
+    <mergeCell ref="AN8"/>
+    <mergeCell ref="AO8"/>
+    <mergeCell ref="AP8"/>
+    <mergeCell ref="AG8"/>
+    <mergeCell ref="AH8"/>
+    <mergeCell ref="AI8"/>
+    <mergeCell ref="AJ8"/>
+    <mergeCell ref="AK8"/>
+    <mergeCell ref="AB8"/>
+    <mergeCell ref="AC8"/>
+    <mergeCell ref="AD8"/>
+    <mergeCell ref="AE8"/>
+    <mergeCell ref="AF8"/>
+    <mergeCell ref="W8"/>
+    <mergeCell ref="X8"/>
+    <mergeCell ref="Y8"/>
+    <mergeCell ref="Z8"/>
+    <mergeCell ref="AA8"/>
+    <mergeCell ref="R8"/>
+    <mergeCell ref="S8"/>
+    <mergeCell ref="T8"/>
+    <mergeCell ref="U8"/>
+    <mergeCell ref="V8"/>
+    <mergeCell ref="M8"/>
+    <mergeCell ref="N8"/>
+    <mergeCell ref="O8"/>
+    <mergeCell ref="P8"/>
+    <mergeCell ref="Q8"/>
     <mergeCell ref="A3:AV3"/>
     <mergeCell ref="A4:AV4"/>
     <mergeCell ref="A5:AV5"/>
@@ -26094,51 +26139,6 @@
     <mergeCell ref="J8"/>
     <mergeCell ref="K8"/>
     <mergeCell ref="L8"/>
-    <mergeCell ref="M8"/>
-    <mergeCell ref="N8"/>
-    <mergeCell ref="O8"/>
-    <mergeCell ref="P8"/>
-    <mergeCell ref="Q8"/>
-    <mergeCell ref="R8"/>
-    <mergeCell ref="S8"/>
-    <mergeCell ref="T8"/>
-    <mergeCell ref="U8"/>
-    <mergeCell ref="V8"/>
-    <mergeCell ref="W8"/>
-    <mergeCell ref="X8"/>
-    <mergeCell ref="Y8"/>
-    <mergeCell ref="Z8"/>
-    <mergeCell ref="AA8"/>
-    <mergeCell ref="AB8"/>
-    <mergeCell ref="AC8"/>
-    <mergeCell ref="AD8"/>
-    <mergeCell ref="AE8"/>
-    <mergeCell ref="AF8"/>
-    <mergeCell ref="AM8"/>
-    <mergeCell ref="AN8"/>
-    <mergeCell ref="AO8"/>
-    <mergeCell ref="AP8"/>
-    <mergeCell ref="AG8"/>
-    <mergeCell ref="AH8"/>
-    <mergeCell ref="AI8"/>
-    <mergeCell ref="AJ8"/>
-    <mergeCell ref="AK8"/>
-    <mergeCell ref="AV8"/>
-    <mergeCell ref="A111:AV111"/>
-    <mergeCell ref="A112:AV112"/>
-    <mergeCell ref="A113:AV113"/>
-    <mergeCell ref="A105:AV105"/>
-    <mergeCell ref="A106:AV106"/>
-    <mergeCell ref="A107:AV107"/>
-    <mergeCell ref="A108:AV108"/>
-    <mergeCell ref="A109:AV109"/>
-    <mergeCell ref="A110:AV110"/>
-    <mergeCell ref="AQ8"/>
-    <mergeCell ref="AR8"/>
-    <mergeCell ref="AS8"/>
-    <mergeCell ref="AT8"/>
-    <mergeCell ref="AU8"/>
-    <mergeCell ref="AL8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
@@ -26243,26 +26243,26 @@
     </row>
     <row r="4" spans="1:24" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="104"/>
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+      <c r="T4" s="104"/>
+      <c r="U4" s="104"/>
       <c r="V4" s="88"/>
       <c r="W4" s="34"/>
       <c r="X4" s="34"/>
@@ -26277,35 +26277,35 @@
         <v>373</v>
       </c>
       <c r="E5" s="94"/>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="105" t="s">
         <v>378</v>
       </c>
-      <c r="G5" s="103"/>
+      <c r="G5" s="105"/>
       <c r="H5" s="93"/>
-      <c r="I5" s="103" t="s">
+      <c r="I5" s="105" t="s">
         <v>375</v>
       </c>
-      <c r="J5" s="103"/>
+      <c r="J5" s="105"/>
       <c r="K5" s="93"/>
-      <c r="L5" s="103" t="s">
+      <c r="L5" s="105" t="s">
         <v>374</v>
       </c>
-      <c r="M5" s="103"/>
+      <c r="M5" s="105"/>
       <c r="N5" s="93"/>
-      <c r="O5" s="103" t="s">
+      <c r="O5" s="105" t="s">
         <v>372</v>
       </c>
-      <c r="P5" s="103"/>
+      <c r="P5" s="105"/>
       <c r="Q5" s="93"/>
-      <c r="R5" s="103" t="s">
+      <c r="R5" s="105" t="s">
         <v>371</v>
       </c>
-      <c r="S5" s="103"/>
+      <c r="S5" s="105"/>
       <c r="T5" s="93"/>
-      <c r="U5" s="103" t="s">
+      <c r="U5" s="105" t="s">
         <v>370</v>
       </c>
-      <c r="V5" s="103"/>
+      <c r="V5" s="105"/>
       <c r="W5" s="50"/>
       <c r="X5" s="50"/>
     </row>
@@ -26857,35 +26857,35 @@
         <v>-1.2E-2</v>
       </c>
       <c r="E17" s="46"/>
-      <c r="F17" s="104">
+      <c r="F17" s="102">
         <v>43.8</v>
       </c>
-      <c r="G17" s="104"/>
+      <c r="G17" s="102"/>
       <c r="H17" s="41"/>
-      <c r="I17" s="104">
+      <c r="I17" s="102">
         <v>68.8</v>
       </c>
-      <c r="J17" s="104"/>
+      <c r="J17" s="102"/>
       <c r="K17" s="41"/>
-      <c r="L17" s="104">
+      <c r="L17" s="102">
         <v>1.2</v>
       </c>
-      <c r="M17" s="104"/>
+      <c r="M17" s="102"/>
       <c r="N17" s="41"/>
-      <c r="O17" s="104">
+      <c r="O17" s="102">
         <v>10.1</v>
       </c>
-      <c r="P17" s="104"/>
+      <c r="P17" s="102"/>
       <c r="Q17" s="42"/>
-      <c r="R17" s="104">
+      <c r="R17" s="102">
         <v>3.4</v>
       </c>
-      <c r="S17" s="104"/>
+      <c r="S17" s="102"/>
       <c r="T17" s="41"/>
-      <c r="U17" s="104">
+      <c r="U17" s="102">
         <v>-3.96</v>
       </c>
-      <c r="V17" s="104"/>
+      <c r="V17" s="102"/>
       <c r="W17" s="34"/>
       <c r="X17" s="34"/>
     </row>
@@ -26899,35 +26899,35 @@
         <v>-1E-3</v>
       </c>
       <c r="E18" s="43"/>
-      <c r="F18" s="105">
+      <c r="F18" s="103">
         <v>45.8</v>
       </c>
-      <c r="G18" s="105"/>
+      <c r="G18" s="103"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="105">
+      <c r="I18" s="103">
         <v>69.5</v>
       </c>
-      <c r="J18" s="105"/>
+      <c r="J18" s="103"/>
       <c r="K18" s="41"/>
-      <c r="L18" s="105">
+      <c r="L18" s="103">
         <v>1.5</v>
       </c>
-      <c r="M18" s="105"/>
+      <c r="M18" s="103"/>
       <c r="N18" s="41"/>
-      <c r="O18" s="105">
+      <c r="O18" s="103">
         <v>12.1</v>
       </c>
-      <c r="P18" s="105"/>
+      <c r="P18" s="103"/>
       <c r="Q18" s="42"/>
-      <c r="R18" s="105">
+      <c r="R18" s="103">
         <v>4.0999999999999996</v>
       </c>
-      <c r="S18" s="105"/>
+      <c r="S18" s="103"/>
       <c r="T18" s="41"/>
-      <c r="U18" s="105">
+      <c r="U18" s="103">
         <v>-2.7</v>
       </c>
-      <c r="V18" s="105"/>
+      <c r="V18" s="103"/>
       <c r="W18" s="34"/>
       <c r="X18" s="34"/>
     </row>
@@ -26941,35 +26941,35 @@
         <v>0.01</v>
       </c>
       <c r="E19" s="43"/>
-      <c r="F19" s="105">
+      <c r="F19" s="103">
         <v>47</v>
       </c>
-      <c r="G19" s="105"/>
+      <c r="G19" s="103"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="105">
+      <c r="I19" s="103">
         <v>71.3</v>
       </c>
-      <c r="J19" s="105"/>
+      <c r="J19" s="103"/>
       <c r="K19" s="41"/>
-      <c r="L19" s="105">
+      <c r="L19" s="103">
         <v>1.8</v>
       </c>
-      <c r="M19" s="105"/>
+      <c r="M19" s="103"/>
       <c r="N19" s="41"/>
-      <c r="O19" s="105">
+      <c r="O19" s="103">
         <v>17.100000000000001</v>
       </c>
-      <c r="P19" s="105"/>
+      <c r="P19" s="103"/>
       <c r="Q19" s="42"/>
-      <c r="R19" s="105">
+      <c r="R19" s="103">
         <v>5.5</v>
       </c>
-      <c r="S19" s="105"/>
+      <c r="S19" s="103"/>
       <c r="T19" s="41"/>
-      <c r="U19" s="105">
+      <c r="U19" s="103">
         <v>-1.53</v>
       </c>
-      <c r="V19" s="105"/>
+      <c r="V19" s="103"/>
       <c r="W19" s="34"/>
       <c r="X19" s="34"/>
     </row>
@@ -27157,6 +27157,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B4:U4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L19:M19"/>
@@ -27169,19 +27182,6 @@
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="R18:S18"/>
     <mergeCell ref="R19:S19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B4:U4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="U5:V5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
@@ -27250,17 +27250,17 @@
     </row>
     <row r="4" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
     </row>
@@ -28159,20 +28159,20 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="30"/>
-    <col min="4" max="4" width="33.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="30" customWidth="1"/>
     <col min="5" max="7" width="11.85546875" style="30" customWidth="1"/>
     <col min="8" max="8" width="1.42578125" style="30" customWidth="1"/>
     <col min="9" max="12" width="11.85546875" style="30" customWidth="1"/>
     <col min="13" max="13" width="1.42578125" style="30" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" style="30" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" style="30" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="30" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" style="30" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
@@ -28203,21 +28203,21 @@
     <row r="9" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
       <c r="C9" s="68"/>
-      <c r="D9" s="121" t="s">
-        <v>418</v>
-      </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="J9" s="120"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
-      <c r="O9" s="120"/>
-      <c r="P9" s="120"/>
+      <c r="D9" s="114" t="s">
+        <v>417</v>
+      </c>
+      <c r="E9" s="115"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
       <c r="Q9" s="68"/>
       <c r="R9" s="68"/>
     </row>
@@ -28234,14 +28234,14 @@
       <c r="G10" s="110"/>
       <c r="H10" s="83"/>
       <c r="I10" s="111" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J10" s="110"/>
       <c r="K10" s="110"/>
       <c r="L10" s="110"/>
       <c r="M10" s="83"/>
-      <c r="N10" s="110" t="s">
-        <v>414</v>
+      <c r="N10" s="111" t="s">
+        <v>418</v>
       </c>
       <c r="O10" s="110"/>
       <c r="P10" s="110"/>
@@ -28266,13 +28266,13 @@
         <v>387</v>
       </c>
       <c r="J11" s="79" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K11" s="79" t="s">
         <v>386</v>
       </c>
       <c r="L11" s="79" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M11" s="80"/>
       <c r="N11" s="79" t="s">

</xml_diff>